<commit_message>
Created pivot table in consolidated cleaned data
</commit_message>
<xml_diff>
--- a/KijahreEstimator_Worksheet.xlsx
+++ b/KijahreEstimator_Worksheet.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CD726A-651B-4208-AAC2-7D346EECD5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D557F8A-7612-4B02-A54D-380166CDCC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Rates" sheetId="4" r:id="rId1"/>
     <sheet name="Summary - Table" sheetId="3" r:id="rId2"/>
     <sheet name="Conduit + Wire - Pricing Calcul" sheetId="1" r:id="rId3"/>
     <sheet name="Conduit + Wire - Table" sheetId="2" r:id="rId4"/>
-    <sheet name="Working Table" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -669,7 +668,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -760,56 +759,18 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -818,17 +779,41 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="7" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -838,12 +823,23 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1192,7 +1188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE616AF9-9B46-461A-A89A-65C9664EBDCF}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
@@ -1230,15 +1226,15 @@
       <c r="G1" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="9" t="s">
@@ -1268,15 +1264,15 @@
         <f>SUM(E2:F2)</f>
         <v>0</v>
       </c>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="9"/>
@@ -1292,15 +1288,15 @@
         <f t="shared" ref="G3:G9" si="1">SUM(E3:F3)</f>
         <v>0</v>
       </c>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="63"/>
+      <c r="O3" s="63"/>
+      <c r="P3" s="63"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="9"/>
@@ -1316,15 +1312,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
-      <c r="K4" s="77"/>
-      <c r="L4" s="77"/>
-      <c r="M4" s="77"/>
-      <c r="N4" s="77"/>
-      <c r="O4" s="77"/>
-      <c r="P4" s="77"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="63"/>
+      <c r="N4" s="63"/>
+      <c r="O4" s="63"/>
+      <c r="P4" s="63"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="9"/>
@@ -1340,15 +1336,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-      <c r="L5" s="77"/>
-      <c r="M5" s="77"/>
-      <c r="N5" s="77"/>
-      <c r="O5" s="77"/>
-      <c r="P5" s="77"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A6" s="9"/>
@@ -1364,15 +1360,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="77"/>
-      <c r="M6" s="77"/>
-      <c r="N6" s="77"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="77"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A7" s="9"/>
@@ -1388,15 +1384,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H7" s="77"/>
-      <c r="I7" s="77"/>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
     </row>
     <row r="8" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9"/>
@@ -1412,382 +1408,372 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="77"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="77"/>
-      <c r="P8" s="77"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="87"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="81"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9" s="77"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="77"/>
-      <c r="K9" s="77"/>
-      <c r="L9" s="77"/>
-      <c r="M9" s="77"/>
-      <c r="N9" s="77"/>
-      <c r="O9" s="77"/>
-      <c r="P9" s="77"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="63"/>
+      <c r="P9" s="63"/>
     </row>
     <row r="10" spans="1:16" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="56"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="54" t="s">
+      <c r="D10" s="14"/>
+      <c r="E10" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="57" t="str">
+      <c r="F10" s="54" t="str">
         <f>C10</f>
         <v>TOTAL</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="G10" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
-      <c r="P10" s="77"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="63"/>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="63"/>
+      <c r="P10" s="63"/>
     </row>
     <row r="11" spans="1:16" ht="18.399999999999999" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59"/>
-      <c r="C11" s="60" t="s">
+      <c r="A11" s="55"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="62" t="s">
+      <c r="D11" s="55"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="58"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="77"/>
-      <c r="N11" s="77"/>
-      <c r="O11" s="77"/>
-      <c r="P11" s="77"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="63"/>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
     </row>
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="65">
+      <c r="B12" s="86">
         <f>SUM(B2:B8)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="65">
+      <c r="C12" s="86">
         <f t="shared" ref="C12:G12" si="2">SUM(C2:C8)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="65">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="65">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="65">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="66">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="78" t="s">
+      <c r="D12" s="86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="73">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="77"/>
-      <c r="O12" s="77"/>
-      <c r="P12" s="77"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="76"/>
+      <c r="L12" s="76"/>
+      <c r="M12" s="76"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="64"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
-      <c r="N13" s="77"/>
-      <c r="O13" s="77"/>
-      <c r="P13" s="77"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76"/>
+      <c r="K13" s="76"/>
+      <c r="L13" s="76"/>
+      <c r="M13" s="76"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="77"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="77"/>
-      <c r="P14" s="77"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
     </row>
     <row r="15" spans="1:16" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="H15" s="77"/>
-      <c r="I15" s="80" t="s">
+      <c r="H15" s="63"/>
+      <c r="I15" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="81">
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="65">
         <f>'Summary - Rates'!B3</f>
         <v>0.3</v>
       </c>
-      <c r="N15" s="77"/>
-      <c r="O15" s="77"/>
-      <c r="P15" s="77"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
     </row>
     <row r="16" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="63"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="82"/>
-      <c r="I16" s="82"/>
-      <c r="J16" s="82"/>
-      <c r="K16" s="82"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82"/>
+      <c r="A16" s="58"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="66"/>
+      <c r="J16" s="66"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A17" s="77"/>
-      <c r="G17" s="77"/>
-      <c r="H17" s="77"/>
-      <c r="I17" s="77"/>
-      <c r="J17" s="77"/>
-      <c r="K17" s="77"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="77"/>
-      <c r="N17" s="77"/>
-      <c r="O17" s="77"/>
-      <c r="P17" s="77"/>
+      <c r="A17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="63"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
     </row>
     <row r="18" spans="1:16" ht="30.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="77"/>
-      <c r="B18" s="68" t="s">
+      <c r="A18" s="63"/>
+      <c r="B18" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="83"/>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
-      <c r="J18" s="83"/>
-      <c r="K18" s="83"/>
-      <c r="L18" s="77"/>
-      <c r="M18" s="77"/>
-      <c r="N18" s="77"/>
-      <c r="O18" s="77"/>
-      <c r="P18" s="77"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
     </row>
     <row r="19" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="77"/>
-      <c r="B19" s="69" t="s">
+      <c r="A19" s="63"/>
+      <c r="B19" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="74"/>
+      <c r="C19" s="70"/>
       <c r="D19" s="71"/>
       <c r="E19" s="71"/>
       <c r="F19" s="71"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="83"/>
-      <c r="I19" s="83"/>
-      <c r="J19" s="83"/>
-      <c r="K19" s="83"/>
-      <c r="L19" s="77"/>
-      <c r="M19" s="77"/>
-      <c r="N19" s="77"/>
-      <c r="O19" s="77"/>
-      <c r="P19" s="77"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
     </row>
     <row r="20" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="77"/>
-      <c r="B20" s="69" t="s">
+      <c r="A20" s="63"/>
+      <c r="B20" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="72"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="70"/>
-      <c r="J20" s="70"/>
-      <c r="K20" s="70"/>
-      <c r="L20" s="77"/>
-      <c r="M20" s="77"/>
-      <c r="N20" s="77"/>
-      <c r="O20" s="77"/>
-      <c r="P20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
     </row>
     <row r="21" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="77"/>
-      <c r="B21" s="69" t="s">
+      <c r="A21" s="63"/>
+      <c r="B21" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="74"/>
+      <c r="C21" s="70"/>
       <c r="D21" s="71"/>
       <c r="E21" s="71"/>
       <c r="F21" s="71"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="83"/>
-      <c r="I21" s="83"/>
-      <c r="J21" s="83"/>
-      <c r="K21" s="83"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="77"/>
-      <c r="N21" s="77"/>
-      <c r="O21" s="77"/>
-      <c r="P21" s="77"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="63"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
     </row>
     <row r="22" spans="1:16" ht="18" x14ac:dyDescent="0.45">
-      <c r="A22" s="77"/>
-      <c r="B22" s="88"/>
-      <c r="C22" s="89"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="83"/>
-      <c r="L22" s="77"/>
-      <c r="M22" s="77"/>
-      <c r="N22" s="77"/>
-      <c r="O22" s="77"/>
-      <c r="P22" s="77"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="69"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="63"/>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A23" s="77"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="90" t="s">
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="90"/>
-      <c r="H23" s="90"/>
-      <c r="I23" s="83"/>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
-      <c r="P23" s="77"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A24" s="77"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="90"/>
-      <c r="F24" s="90"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="90"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="77"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="77"/>
-      <c r="P24" s="77"/>
+      <c r="A24" s="63"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="63"/>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="63"/>
+      <c r="P24" s="63"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A25" s="77"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="77"/>
-      <c r="P25" s="77"/>
+      <c r="A25" s="63"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="63"/>
+      <c r="L25" s="63"/>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A26" s="77"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
+      <c r="A26" s="63"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
+      <c r="L26" s="63"/>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C23:H25"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:M13"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:K20"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
@@ -1797,6 +1783,13 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C23:H25"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:M13"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2708,7 +2701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC8A70E-28A6-45FE-BB15-B1F24572711E}">
   <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -4512,18 +4505,4 @@
     <ignoredError sqref="E2:E50 G2:G5" formula="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78246A1E-8505-483A-8DD2-85EF00CB17FA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>